<commit_message>
3D Title Screen :)
</commit_message>
<xml_diff>
--- a/Documents/Hero's Run Revisited.xlsx
+++ b/Documents/Hero's Run Revisited.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="90">
   <si>
     <t>Description</t>
   </si>
@@ -239,6 +239,63 @@
   </si>
   <si>
     <t>Analytics</t>
+  </si>
+  <si>
+    <t>End of game cut-scene</t>
+  </si>
+  <si>
+    <t>4-post bed, or bench</t>
+  </si>
+  <si>
+    <t>Gloves glow when an enemy is around or when a power up is used</t>
+  </si>
+  <si>
+    <t>Hero stats</t>
+  </si>
+  <si>
+    <t>Number of times revived, time to complete, etc</t>
+  </si>
+  <si>
+    <t>Connect to FB reminder popup</t>
+  </si>
+  <si>
+    <t>Video replay</t>
+  </si>
+  <si>
+    <t>Everyplay, ReplayKit for IOS</t>
+  </si>
+  <si>
+    <t>More hero model options</t>
+  </si>
+  <si>
+    <t>Hero's look customizable</t>
+  </si>
+  <si>
+    <t>Secret lair Easter egg</t>
+  </si>
+  <si>
+    <t>Runes light up when enemies are nearby, or you are in heroic or legendary modes or you have purchased the coin doubler, or you are using a power-up</t>
+  </si>
+  <si>
+    <t>Ziplining</t>
+  </si>
+  <si>
+    <t>Endless, distance-based mode that gets unlocked after main quest is completed</t>
+  </si>
+  <si>
+    <t>Collect for Runes to be able to activate Cullis Gate</t>
+  </si>
+  <si>
+    <t>Loading Menu tips</t>
+  </si>
+  <si>
+    <t>Fortune Teller gipsy caravan</t>
+  </si>
+  <si>
+    <t>Subsribe to newsletter, get quirky horoscope</t>
+  </si>
+  <si>
+    <t>Keep troll as pursuier or simply use as an enemy?</t>
   </si>
 </sst>
 </file>
@@ -309,7 +366,9 @@
     </border>
   </borders>
   <cellStyleXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -328,19 +387,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -359,7 +426,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -688,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -700,6 +767,7 @@
     <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="23">
@@ -718,8 +786,16 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="75">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -751,10 +827,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -923,7 +999,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -972,7 +1048,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" ht="30">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1007,6 +1083,11 @@
         <v>69</v>
       </c>
     </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>59</v>
@@ -1037,39 +1118,103 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="30">
+      <c r="A47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30">
+      <c r="A49" t="s">
+        <v>87</v>
+      </c>
+      <c r="F49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30">
+      <c r="A50" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1089,7 +1234,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1180,32 +1325,40 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:6">
       <c r="A33" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:6">
       <c r="A36" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="6" customFormat="1">
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="6" customFormat="1">
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1231,17 +1384,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="75">
       <c r="A2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" ht="75">
       <c r="A3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" ht="30">
       <c r="A4" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Endless mode - post-level popup draft version
</commit_message>
<xml_diff>
--- a/Documents/Hero's Run Revisited.xlsx
+++ b/Documents/Hero's Run Revisited.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
   <si>
     <t>Description</t>
   </si>
@@ -296,6 +296,75 @@
   </si>
   <si>
     <t>Keep troll as pursuier or simply use as an enemy?</t>
+  </si>
+  <si>
+    <t>Dynamic music</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Play combat music when there are enemies around</t>
+  </si>
+  <si>
+    <t>Macaw</t>
+  </si>
+  <si>
+    <t>Endless runner mode</t>
+  </si>
+  <si>
+    <t>Make tiles inactive after t-junction</t>
+  </si>
+  <si>
+    <t>Keep only one tile per type in recycle list and try destroying others</t>
+  </si>
+  <si>
+    <t>Add stumbles: roots and rocks</t>
+  </si>
+  <si>
+    <t>Add objects in middlle of the path</t>
+  </si>
+  <si>
+    <t>Add a way to tag tiles as suitable for endless running with a weight system</t>
+  </si>
+  <si>
+    <t>isLandmark, isGoodForEndless, probability of apperance</t>
+  </si>
+  <si>
+    <t>New personal high score message in-game</t>
+  </si>
+  <si>
+    <t>Have a high score per theme</t>
+  </si>
+  <si>
+    <t>Have a leaderboard on gamecenter per theme</t>
+  </si>
+  <si>
+    <t>Have a challenge a friend mode</t>
+  </si>
+  <si>
+    <t>also challenge non-app users</t>
+  </si>
+  <si>
+    <t>Code Message center - display challenges and lives received</t>
+  </si>
+  <si>
+    <t>Code new pre-level popup</t>
+  </si>
+  <si>
+    <t>Code new post-level popup</t>
+  </si>
+  <si>
+    <t>Code new save me popup</t>
+  </si>
+  <si>
+    <t>Code selecting theme for endless running</t>
+  </si>
+  <si>
+    <t>Maybe as a scrollable bar</t>
+  </si>
+  <si>
+    <t>Inform user when he has completed an episode, that it is now unlocked for endless running</t>
   </si>
 </sst>
 </file>
@@ -386,7 +455,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -407,6 +476,12 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -827,10 +902,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -840,7 +915,7 @@
     <col min="3" max="3" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="32" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="23">
@@ -859,7 +934,7 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -985,236 +1060,329 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30">
-      <c r="A13" t="s">
+    <row r="14" spans="1:6" ht="30">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" s="10" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3">
-        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>29</v>
+      <c r="C15" s="3">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="8" t="s">
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="30">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30">
-      <c r="A40" t="s">
+    <row r="41" spans="1:6" ht="30">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" s="10" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="F41" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30">
-      <c r="A46" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30">
       <c r="A47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30">
+      <c r="A48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="30">
-      <c r="A49" t="s">
-        <v>87</v>
-      </c>
-      <c r="F49" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30">
       <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30">
+      <c r="A51" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="30">
+      <c r="A55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="30">
+      <c r="A56" t="s">
+        <v>99</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="30">
+      <c r="A59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>104</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="30">
+      <c r="A61" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>110</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="45">
+      <c r="A66" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1233,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1313,6 +1481,21 @@
     <row r="22" spans="1:1">
       <c r="A22" s="8" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:1">

</xml_diff>